<commit_message>
statement instead of question
</commit_message>
<xml_diff>
--- a/inst/extdata/exercises.xlsx
+++ b/inst/extdata/exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joses\Documents\_trabajo\packages\rexer\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AEC945-CD68-4161-8CEA-8AA05729A074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5CB368-D42F-4B92-A8F2-F6B5EB3751BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>question</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>1.LTU, 2.DMA, 3.VCT&lt;|&gt;1.URY, 2.MLI, 3.PRY&lt;|&gt;1.MEX, 2.BFA, 3.BLZ&lt;|&gt;1.GAB, 2.BDI, 3.KGZ</t>
+  </si>
+  <si>
+    <t>statement</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
   <autoFilter ref="A1:H9" xr:uid="{12F42F2D-6E43-4E69-B88B-49F8108A5AE1}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4800CD23-D0A5-4135-9012-8354E0D88484}" name="type"/>
-    <tableColumn id="2" xr3:uid="{66BA156C-96AE-4A8A-AEAB-E16828283CF1}" name="question"/>
+    <tableColumn id="2" xr3:uid="{66BA156C-96AE-4A8A-AEAB-E16828283CF1}" name="statement"/>
     <tableColumn id="3" xr3:uid="{076505AD-0808-44F4-891B-0437F91DAFAE}" name="image"/>
     <tableColumn id="4" xr3:uid="{61796249-F6A8-4CC4-AE72-5F87216BCCC2}" name="image_alt"/>
     <tableColumn id="5" xr3:uid="{A1BCEAE0-BFA8-42B7-885B-55C47C878C03}" name="answer"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,137 +449,137 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>